<commit_message>
Modifications to 9 comparisons file
</commit_message>
<xml_diff>
--- a/9Comparison.xlsx
+++ b/9Comparison.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/WV_SortingNetworks/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="24240" windowHeight="13740" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="24240" windowHeight="13740" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SN_difference9" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="SN2-9_RunTime" sheetId="3" r:id="rId3"/>
     <sheet name="R_Size9&amp;10" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -77,11 +82,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.0000000%"/>
-    <numFmt numFmtId="171" formatCode="0.00000"/>
-    <numFmt numFmtId="173" formatCode="0.000%"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.0000000%"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.000%"/>
+    <numFmt numFmtId="168" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -242,7 +247,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -254,10 +259,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -267,16 +272,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Komma" xfId="2" builtinId="3"/>
+    <cellStyle name="Procent" xfId="1" builtinId="5"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -642,14 +647,14 @@
       <selection activeCell="C2" sqref="C2:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
@@ -989,7 +994,7 @@
         <v>0.99912265309703452</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="8">
         <v>1107</v>
@@ -1006,7 +1011,7 @@
         <v>0.99909665763324296</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="8">
         <v>250</v>
@@ -1023,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="8">
         <v>73</v>
@@ -1040,7 +1045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="8">
         <v>27</v>
@@ -1057,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="8">
         <v>8</v>
@@ -1074,7 +1079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="8">
         <v>1</v>
@@ -1091,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>4</v>
       </c>
@@ -1144,13 +1149,13 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="13" t="s">
         <v>10</v>
       </c>
@@ -1164,7 +1169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
@@ -1185,7 +1190,7 @@
       </c>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -1216,16 +1221,16 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1251,7 +1256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1284,7 +1289,7 @@
         <v>15135.358007399</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1317,7 +1322,7 @@
         <v>15135358.007399</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1343,7 +1348,7 @@
         <v>15135358007399</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H6" s="19"/>
     </row>
   </sheetData>
@@ -1359,13 +1364,13 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1373,7 +1378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -1381,7 +1386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="20">
         <v>3</v>
       </c>
@@ -1389,7 +1394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
         <v>7</v>
       </c>
@@ -1397,7 +1402,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="20">
         <v>20</v>
       </c>
@@ -1405,7 +1410,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="20">
         <v>59</v>
       </c>
@@ -1413,7 +1418,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
         <v>208</v>
       </c>
@@ -1421,7 +1426,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="20">
         <v>807</v>
       </c>
@@ -1429,7 +1434,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="20">
         <v>3415</v>
       </c>
@@ -1437,7 +1442,7 @@
         <v>3996</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="20">
         <v>14340</v>
       </c>
@@ -1445,7 +1450,7 @@
         <v>20125</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="20">
         <v>55986</v>
       </c>
@@ -1453,7 +1458,7 @@
         <v>105335</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="20">
         <v>188710</v>
       </c>
@@ -1461,97 +1466,97 @@
         <v>544875</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>490288</v>
       </c>
       <c r="B13" s="18"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
         <v>854645</v>
       </c>
       <c r="B14" s="18"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="20">
         <v>914533</v>
       </c>
       <c r="B15" s="18"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="20">
         <v>607155</v>
       </c>
       <c r="B16" s="18"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="20">
         <v>274184</v>
       </c>
       <c r="B17" s="18"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="20">
         <v>94080</v>
       </c>
       <c r="B18" s="18"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="20">
         <v>25783</v>
       </c>
       <c r="B19" s="18"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="20">
         <v>5694</v>
       </c>
       <c r="B20" s="18"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="20">
         <v>1106</v>
       </c>
       <c r="B21" s="18"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="20">
         <v>250</v>
       </c>
       <c r="B22" s="18"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="20">
         <v>73</v>
       </c>
       <c r="B23" s="18"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="20">
         <v>27</v>
       </c>
       <c r="B24" s="18"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="20">
         <v>8</v>
       </c>
       <c r="B25" s="18"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="20">
         <v>1</v>
       </c>
       <c r="B26" s="18"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="18"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" s="18"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new pictures in the Excel file
</commit_message>
<xml_diff>
--- a/9Comparison.xlsx
+++ b/9Comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="SN_difference9" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="SN9_RunTime" sheetId="2" r:id="rId6"/>
     <sheet name="Grafiek2" sheetId="6" r:id="rId7"/>
     <sheet name="Grafiek3" sheetId="7" r:id="rId8"/>
-    <sheet name="Grafiek4" sheetId="8" r:id="rId9"/>
+    <sheet name="Grafiek4" sheetId="13" r:id="rId9"/>
     <sheet name="SN2-9_RunTime" sheetId="3" r:id="rId10"/>
     <sheet name="Grafiek5" sheetId="9" r:id="rId11"/>
     <sheet name="R_Size9&amp;10" sheetId="4" r:id="rId12"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Paper</t>
   </si>
@@ -61,15 +61,6 @@
     <t>s</t>
   </si>
   <si>
-    <t>ms</t>
-  </si>
-  <si>
-    <t>Wij</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
     <t>wij/paper</t>
   </si>
   <si>
@@ -84,6 +75,32 @@
   <si>
     <t>channels 10</t>
   </si>
+  <si>
+    <t>Sorteernetwerk 9 kanalen</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Codish </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>et al.
+(288 threads)</t>
+    </r>
+  </si>
+  <si>
+    <t>Dekempeneer &amp; Derkinderen
+(20 threads)</t>
+  </si>
+  <si>
+    <t>Aantal kanalen</t>
+  </si>
 </sst>
 </file>
 
@@ -92,10 +109,10 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="0.0000000%"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
-    <numFmt numFmtId="168" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +133,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -275,14 +299,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="2" builtinId="3"/>
@@ -422,7 +446,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>h</c:v>
+                  <c:v>Sorteernetwerk 9 kanalen</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -514,10 +538,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Wij</c:v>
+                  <c:v>Dekempeneer &amp; Derkinderen_x000d_(20 threads)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Paper</c:v>
+                  <c:v>Codish et al._x000d_(288 threads)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -532,14 +556,13 @@
                   <c:v>4.204722</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>737.9666666666667</c:v>
+                  <c:v>305.9666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -549,11 +572,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="-2061955312"/>
-        <c:axId val="-2060961312"/>
+        <c:axId val="-2125716544"/>
+        <c:axId val="-2125713168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2061955312"/>
+        <c:axId val="-2125716544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -591,7 +614,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2060961312"/>
+        <c:crossAx val="-2125713168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -599,7 +622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2060961312"/>
+        <c:axId val="-2125713168"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -651,7 +674,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2061955312"/>
+        <c:crossAx val="-2125716544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -803,7 +826,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>h</c:v>
+                  <c:v>Sorteernetwerk 9 kanalen</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -895,10 +918,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Wij</c:v>
+                  <c:v>Dekempeneer &amp; Derkinderen_x000d_(20 threads)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Paper</c:v>
+                  <c:v>Codish et al._x000d_(288 threads)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -913,7 +936,7 @@
                   <c:v>4.204722</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>737.9666666666667</c:v>
+                  <c:v>305.9666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -929,11 +952,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="41"/>
-        <c:axId val="-2106542352"/>
-        <c:axId val="-2090806400"/>
+        <c:axId val="-2128365920"/>
+        <c:axId val="-2128366464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2106542352"/>
+        <c:axId val="-2128365920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,7 +994,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090806400"/>
+        <c:crossAx val="-2128366464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -979,7 +1002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2090806400"/>
+        <c:axId val="-2128366464"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -990,7 +1013,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2106542352"/>
+        <c:crossAx val="-2128365920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1063,6 +1086,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Avenir Next" charset="0"/>
+                <a:ea typeface="Avenir Next" charset="0"/>
+                <a:cs typeface="Avenir Next" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1">
+                <a:latin typeface="Avenir Next" charset="0"/>
+                <a:ea typeface="Avenir Next" charset="0"/>
+                <a:cs typeface="Avenir Next" charset="0"/>
+              </a:rPr>
+              <a:t>Uitvoeringstijd algoritme</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1077,16 +1129,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="Avenir Next" charset="0"/>
+              <a:ea typeface="Avenir Next" charset="0"/>
+              <a:cs typeface="Avenir Next" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="nl-NL"/>
@@ -1109,7 +1161,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>h</c:v>
+                  <c:v>Sorteernetwerk 9 kanalen</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1124,16 +1176,74 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Avenir Next" charset="0"/>
+                    <a:ea typeface="Avenir Next" charset="0"/>
+                    <a:cs typeface="Avenir Next" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>SN9_RunTime!$A$2:$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Wij</c:v>
+                  <c:v>Dekempeneer &amp; Derkinderen_x000d_(20 threads)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Paper</c:v>
+                  <c:v>Codish et al._x000d_(288 threads)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1148,7 +1258,7 @@
                   <c:v>4.204722</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>737.9666666666667</c:v>
+                  <c:v>305.9666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1156,19 +1266,18 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-2108007728"/>
-        <c:axId val="-2092560960"/>
+        <c:gapWidth val="75"/>
+        <c:axId val="-2128384048"/>
+        <c:axId val="-2128387408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2108007728"/>
+        <c:axId val="-2128384048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1196,22 +1305,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Avenir Next" charset="0"/>
+                <a:ea typeface="Avenir Next" charset="0"/>
+                <a:cs typeface="Avenir Next" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2092560960"/>
+        <c:crossAx val="-2128387408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1219,30 +1328,76 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2092560960"/>
+        <c:axId val="-2128387408"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Avenir Next" charset="0"/>
+                    <a:ea typeface="Avenir Next" charset="0"/>
+                    <a:cs typeface="Avenir Next" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL" sz="1200" b="1">
+                    <a:latin typeface="Avenir Next" charset="0"/>
+                    <a:ea typeface="Avenir Next" charset="0"/>
+                    <a:cs typeface="Avenir Next" charset="0"/>
+                  </a:rPr>
+                  <a:t>Tijd [uur]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Avenir Next" charset="0"/>
+                  <a:ea typeface="Avenir Next" charset="0"/>
+                  <a:cs typeface="Avenir Next" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1258,22 +1413,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Avenir Next" charset="0"/>
+                <a:ea typeface="Avenir Next" charset="0"/>
+                <a:cs typeface="Avenir Next" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2108007728"/>
+        <c:crossAx val="-2128384048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1285,6 +1440,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Avenir Next" charset="0"/>
+              <a:ea typeface="Avenir Next" charset="0"/>
+              <a:cs typeface="Avenir Next" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1378,7 +1565,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>h</c:v>
+                  <c:v>Sorteernetwerk 9 kanalen</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1399,10 +1586,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Wij</c:v>
+                  <c:v>Dekempeneer &amp; Derkinderen_x000d_(20 threads)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Paper</c:v>
+                  <c:v>Codish et al._x000d_(288 threads)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1417,7 +1604,7 @@
                   <c:v>4.204722</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>737.9666666666667</c:v>
+                  <c:v>305.9666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1433,11 +1620,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2096268640"/>
-        <c:axId val="2134354416"/>
+        <c:axId val="-2129789520"/>
+        <c:axId val="-2129786112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2096268640"/>
+        <c:axId val="-2129789520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1480,7 +1667,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134354416"/>
+        <c:crossAx val="-2129786112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1488,7 +1675,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134354416"/>
+        <c:axId val="-2129786112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,7 +1728,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096268640"/>
+        <c:crossAx val="-2129789520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1726,11 +1913,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2095620976"/>
-        <c:axId val="-2091488480"/>
+        <c:axId val="-2125576592"/>
+        <c:axId val="-2125573200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2095620976"/>
+        <c:axId val="-2125576592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1773,7 +1960,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2091488480"/>
+        <c:crossAx val="-2125573200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1781,7 +1968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2091488480"/>
+        <c:axId val="-2125573200"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1833,7 +2020,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2095620976"/>
+        <c:crossAx val="-2125576592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2050,11 +2237,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2108855664"/>
-        <c:axId val="-2110848480"/>
+        <c:axId val="-2125533440"/>
+        <c:axId val="-2125530048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2108855664"/>
+        <c:axId val="-2125533440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2097,7 +2284,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2110848480"/>
+        <c:crossAx val="-2125530048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2105,7 +2292,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110848480"/>
+        <c:axId val="-2125530048"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2157,7 +2344,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2108855664"/>
+        <c:crossAx val="-2125533440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2294,7 +2481,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ms</c:v>
+                  <c:v>Aantal kanalen</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2309,6 +2496,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Avenir Next" charset="0"/>
+                    <a:ea typeface="Avenir Next" charset="0"/>
+                    <a:cs typeface="Avenir Next" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>'SN2-9_RunTime'!$C$1:$H$1</c:f>
@@ -2338,29 +2583,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SN2-9_RunTime'!$A$3:$H$3</c:f>
+              <c:f>'SN2-9_RunTime'!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16.933678</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.933678</c:v>
+                  <c:v>25.051018</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.051018</c:v>
+                  <c:v>82.439151</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82.439151</c:v>
+                  <c:v>141.477278</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>141.477278</c:v>
+                  <c:v>6680.307154</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6680.307154</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>1.5135358007399E7</c:v>
                 </c:pt>
               </c:numCache>
@@ -2369,19 +2611,18 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-2094045600"/>
-        <c:axId val="-2106880752"/>
+        <c:gapWidth val="75"/>
+        <c:axId val="-2081507504"/>
+        <c:axId val="-2063279936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2094045600"/>
+        <c:axId val="-2081507504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2409,22 +2650,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Avenir Next" charset="0"/>
+                <a:ea typeface="Avenir Next" charset="0"/>
+                <a:cs typeface="Avenir Next" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2106880752"/>
+        <c:crossAx val="-2063279936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2432,35 +2673,83 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2106880752"/>
+        <c:axId val="-2063279936"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL" sz="1200" b="1">
+                    <a:latin typeface="Avenir Next" charset="0"/>
+                    <a:ea typeface="Avenir Next" charset="0"/>
+                    <a:cs typeface="Avenir Next" charset="0"/>
+                  </a:rPr>
+                  <a:t>Tijd [miliseconde]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2469,22 +2758,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Avenir Next" charset="0"/>
+                <a:ea typeface="Avenir Next" charset="0"/>
+                <a:cs typeface="Avenir Next" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2094045600"/>
+        <c:crossAx val="-2081507504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2512,16 +2801,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="Avenir Next" charset="0"/>
+              <a:ea typeface="Avenir Next" charset="0"/>
+              <a:cs typeface="Avenir Next" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="nl-NL"/>
@@ -2575,7 +2864,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2798,11 +3086,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2090529648"/>
-        <c:axId val="-2092558384"/>
+        <c:axId val="-2128493072"/>
+        <c:axId val="-2128496352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2090529648"/>
+        <c:axId val="-2128493072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2845,7 +3133,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2092558384"/>
+        <c:crossAx val="-2128496352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2853,7 +3141,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2092558384"/>
+        <c:axId val="-2128496352"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2905,7 +3193,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090529648"/>
+        <c:crossAx val="-2128493072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2919,7 +3207,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7457,7 +7744,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="109" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7468,7 +7755,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="109" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7545,7 +7832,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309340" cy="6074434"/>
+    <xdr:ext cx="9321101" cy="6082018"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -7572,7 +7859,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309340" cy="6074434"/>
+    <xdr:ext cx="9321101" cy="6082018"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -7599,7 +7886,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309340" cy="6074434"/>
+    <xdr:ext cx="9321101" cy="6082018"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -7626,7 +7913,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309340" cy="6074434"/>
+    <xdr:ext cx="9321101" cy="6082018"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -7653,7 +7940,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309340" cy="6074434"/>
+    <xdr:ext cx="9321101" cy="6082018"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -7680,7 +7967,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309340" cy="6074434"/>
+    <xdr:ext cx="9321101" cy="6082018"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -7707,7 +7994,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309340" cy="6074434"/>
+    <xdr:ext cx="9321101" cy="6082018"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -8549,12 +8836,13 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
@@ -8563,7 +8851,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>6</v>
@@ -8572,45 +8860,45 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="16">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="15">
         <v>4.2047220000000003</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="15">
         <f>$B2*60</f>
         <v>252.28332</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="15">
         <f>$C2*60</f>
         <v>15136.9992</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <f>D2/D3</f>
-        <v>5.6977126338136324E-3</v>
-      </c>
-      <c r="G2" s="15"/>
+        <v>1.3742418564113738E-2</v>
+      </c>
+      <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="16">
-        <f>(7*60 + 17 + 58/60) + 5*60</f>
-        <v>737.9666666666667</v>
-      </c>
-      <c r="C3" s="16">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="15">
+        <f>(7*24 + 17 + 58/60) + 5*24</f>
+        <v>305.9666666666667</v>
+      </c>
+      <c r="C3" s="15">
         <f>$B3*60</f>
-        <v>44278</v>
-      </c>
-      <c r="D3" s="16">
+        <v>18358</v>
+      </c>
+      <c r="D3" s="15">
         <f>$C3*60</f>
-        <v>2656680</v>
+        <v>1101480</v>
       </c>
     </row>
   </sheetData>
@@ -8623,8 +8911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8640,7 +8928,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1">
         <v>3</v>
@@ -8668,96 +8956,96 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="15">
         <f>B$3/1000</f>
         <v>9.1420945000000003E-2</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="15">
         <f t="shared" ref="C2:H2" si="0">C$3/1000</f>
         <v>1.6933678000000001E-2</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="15">
         <f t="shared" si="0"/>
         <v>2.5051017999999998E-2</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="15">
         <f t="shared" si="0"/>
         <v>8.2439151000000002E-2</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="15">
         <f t="shared" si="0"/>
         <v>0.14147727800000001</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="15">
         <f t="shared" si="0"/>
         <v>6.6803071540000003</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="15">
         <f t="shared" si="0"/>
         <v>15135.358007399</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="16">
+        <v>16</v>
+      </c>
+      <c r="B3" s="15">
         <f>B$4/1000000</f>
         <v>91.420945000000003</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <f t="shared" ref="C3:H3" si="1">C$4/1000000</f>
         <v>16.933678</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <f t="shared" si="1"/>
         <v>25.051017999999999</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <f t="shared" si="1"/>
         <v>82.439150999999995</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="15">
         <f t="shared" si="1"/>
         <v>141.47727800000001</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="15">
         <f t="shared" si="1"/>
         <v>6680.3071540000001</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <f t="shared" si="1"/>
         <v>15135358.007399</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="17">
+        <v>9</v>
+      </c>
+      <c r="B4" s="16">
         <v>91420945</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
         <v>16933678</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>25051018</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>82439151</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>141477278</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>6680307154</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <v>15135358007399</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H6" s="18"/>
+      <c r="H6" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8781,192 +9069,192 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="19">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="19">
+      <c r="A3" s="18">
         <v>3</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="19">
+      <c r="A4" s="18">
         <v>7</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="19">
+      <c r="A5" s="18">
         <v>20</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="19">
+      <c r="A6" s="18">
         <v>59</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <v>208</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="19">
+      <c r="A8" s="18">
         <v>807</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <v>864</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="19">
+      <c r="A9" s="18">
         <v>3415</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>3996</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="19">
+      <c r="A10" s="18">
         <v>14340</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="16">
         <v>20125</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="19">
+      <c r="A11" s="18">
         <v>55986</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>105335</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="19">
+      <c r="A12" s="18">
         <v>188710</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>544875</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="19">
+      <c r="A13" s="18">
         <v>490288</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="16"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="19">
+      <c r="A14" s="18">
         <v>854645</v>
       </c>
-      <c r="B14" s="17"/>
+      <c r="B14" s="16"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="19">
+      <c r="A15" s="18">
         <v>914533</v>
       </c>
-      <c r="B15" s="17"/>
+      <c r="B15" s="16"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="19">
+      <c r="A16" s="18">
         <v>607155</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="16"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="19">
+      <c r="A17" s="18">
         <v>274184</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="16"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="19">
+      <c r="A18" s="18">
         <v>94080</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="16"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="19">
+      <c r="A19" s="18">
         <v>25783</v>
       </c>
-      <c r="B19" s="17"/>
+      <c r="B19" s="16"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="19">
+      <c r="A20" s="18">
         <v>5694</v>
       </c>
-      <c r="B20" s="17"/>
+      <c r="B20" s="16"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="19">
+      <c r="A21" s="18">
         <v>1106</v>
       </c>
-      <c r="B21" s="17"/>
+      <c r="B21" s="16"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="19">
+      <c r="A22" s="18">
         <v>250</v>
       </c>
-      <c r="B22" s="17"/>
+      <c r="B22" s="16"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="19">
+      <c r="A23" s="18">
         <v>73</v>
       </c>
-      <c r="B23" s="17"/>
+      <c r="B23" s="16"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="19">
+      <c r="A24" s="18">
         <v>27</v>
       </c>
-      <c r="B24" s="17"/>
+      <c r="B24" s="16"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="19">
+      <c r="A25" s="18">
         <v>8</v>
       </c>
-      <c r="B25" s="17"/>
+      <c r="B25" s="16"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="19">
+      <c r="A26" s="18">
         <v>1</v>
       </c>
-      <c r="B26" s="17"/>
+      <c r="B26" s="16"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="17"/>
+      <c r="B27" s="16"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="17"/>
+      <c r="B28" s="16"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="17"/>
+      <c r="B29" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated poster + excel
</commit_message>
<xml_diff>
--- a/9Comparison.xlsx
+++ b/9Comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="SN_difference9" sheetId="1" r:id="rId1"/>
@@ -399,7 +399,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -514,7 +513,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -572,11 +570,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="-2125716544"/>
-        <c:axId val="-2125713168"/>
+        <c:axId val="2126782624"/>
+        <c:axId val="2125676976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125716544"/>
+        <c:axId val="2126782624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -614,7 +612,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125713168"/>
+        <c:crossAx val="2125676976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -622,7 +620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125713168"/>
+        <c:axId val="2125676976"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -674,7 +672,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125716544"/>
+        <c:crossAx val="2126782624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -688,7 +686,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -779,7 +776,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -894,7 +890,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -952,11 +947,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="41"/>
-        <c:axId val="-2128365920"/>
-        <c:axId val="-2128366464"/>
+        <c:axId val="2125944208"/>
+        <c:axId val="2125947584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2128365920"/>
+        <c:axId val="2125944208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -994,7 +989,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128366464"/>
+        <c:crossAx val="2125947584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1002,7 +997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128366464"/>
+        <c:axId val="2125947584"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1013,7 +1008,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128365920"/>
+        <c:crossAx val="2125944208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1115,7 +1110,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1215,7 +1209,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1273,11 +1266,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="-2128384048"/>
-        <c:axId val="-2128387408"/>
+        <c:axId val="2125999552"/>
+        <c:axId val="2126002896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2128384048"/>
+        <c:axId val="2125999552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,7 +1313,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128387408"/>
+        <c:crossAx val="2126002896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1328,7 +1321,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128387408"/>
+        <c:axId val="2126002896"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1365,7 +1358,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1428,7 +1420,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128384048"/>
+        <c:crossAx val="2125999552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1442,7 +1434,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1519,7 +1510,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1620,11 +1610,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2129789520"/>
-        <c:axId val="-2129786112"/>
+        <c:axId val="2126844320"/>
+        <c:axId val="2126847728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129789520"/>
+        <c:axId val="2126844320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1667,7 +1657,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129786112"/>
+        <c:crossAx val="2126847728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1675,7 +1665,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129786112"/>
+        <c:axId val="2126847728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1728,7 +1718,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129789520"/>
+        <c:crossAx val="2126844320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1787,7 +1777,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1913,11 +1902,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2125576592"/>
-        <c:axId val="-2125573200"/>
+        <c:axId val="2126892928"/>
+        <c:axId val="2126896320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125576592"/>
+        <c:axId val="2126892928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1960,7 +1949,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125573200"/>
+        <c:crossAx val="2126896320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1968,7 +1957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125573200"/>
+        <c:axId val="2126896320"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2020,7 +2009,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125576592"/>
+        <c:crossAx val="2126892928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2034,7 +2023,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2111,7 +2099,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2237,11 +2224,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2125533440"/>
-        <c:axId val="-2125530048"/>
+        <c:axId val="2126934752"/>
+        <c:axId val="2126938144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125533440"/>
+        <c:axId val="2126934752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2284,7 +2271,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125530048"/>
+        <c:crossAx val="2126938144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2292,7 +2279,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125530048"/>
+        <c:axId val="2126938144"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2344,7 +2331,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125533440"/>
+        <c:crossAx val="2126934752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2358,7 +2345,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2462,6 +2448,32 @@
               <a:t>Uitvoeringstijd algoritme</a:t>
             </a:r>
           </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1">
+                <a:latin typeface="Avenir Next" charset="0"/>
+                <a:ea typeface="Avenir Next" charset="0"/>
+                <a:cs typeface="Avenir Next" charset="0"/>
+              </a:rPr>
+              <a:t>Dekempeneer</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
+                <a:latin typeface="Avenir Next" charset="0"/>
+                <a:ea typeface="Avenir Next" charset="0"/>
+                <a:cs typeface="Avenir Next" charset="0"/>
+              </a:rPr>
+              <a:t> &amp; Derkinderen</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600" b="1">
+              <a:latin typeface="Avenir Next" charset="0"/>
+              <a:ea typeface="Avenir Next" charset="0"/>
+              <a:cs typeface="Avenir Next" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
@@ -2647,11 +2659,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="-2081507504"/>
-        <c:axId val="-2063279936"/>
+        <c:axId val="2126983184"/>
+        <c:axId val="2126986512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2081507504"/>
+        <c:axId val="2126983184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2694,7 +2706,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2063279936"/>
+        <c:crossAx val="2126986512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2702,7 +2714,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2063279936"/>
+        <c:axId val="2126986512"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2802,7 +2814,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2081507504"/>
+        <c:crossAx val="2126983184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3115,11 +3127,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2128493072"/>
-        <c:axId val="-2128496352"/>
+        <c:axId val="2127031584"/>
+        <c:axId val="2127034912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2128493072"/>
+        <c:axId val="2127031584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3162,7 +3174,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128496352"/>
+        <c:crossAx val="2127034912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3170,7 +3182,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128496352"/>
+        <c:axId val="2127034912"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3222,7 +3234,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128493072"/>
+        <c:crossAx val="2127031584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7839,7 +7851,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updated comparison 9 channels by new results of VSC
</commit_message>
<xml_diff>
--- a/9Comparison.xlsx
+++ b/9Comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SN_difference9" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Paper</t>
   </si>
@@ -100,6 +100,11 @@
   </si>
   <si>
     <t>Aantal kanalen</t>
+  </si>
+  <si>
+    <t>Algoritme Codish et al. door
+Dekempeneer &amp; Derkinderen
+(20 threads)</t>
   </si>
 </sst>
 </file>
@@ -532,13 +537,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>SN9_RunTime!$A$2:$A$3</c:f>
+              <c:f>SN9_RunTime!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Dekempeneer &amp; Derkinderen_x000d_(20 threads)</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Algoritme Codish et al. door_x000d_Dekempeneer &amp; Derkinderen_x000d_(20 threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Codish et al._x000d_(288 threads)</c:v>
                 </c:pt>
               </c:strCache>
@@ -546,14 +554,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SN9_RunTime!$B$2:$B$3</c:f>
+              <c:f>SN9_RunTime!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>4.204722</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>6.196933330409722</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>305.9666666666667</c:v>
                 </c:pt>
               </c:numCache>
@@ -570,11 +581,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="2126782624"/>
-        <c:axId val="2125676976"/>
+        <c:axId val="2132212384"/>
+        <c:axId val="2132206800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126782624"/>
+        <c:axId val="2132212384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +623,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125676976"/>
+        <c:crossAx val="2132206800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -620,7 +631,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125676976"/>
+        <c:axId val="2132206800"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -672,7 +683,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126782624"/>
+        <c:crossAx val="2132212384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -776,6 +787,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -890,6 +902,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -909,13 +922,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>SN9_RunTime!$A$2:$A$3</c:f>
+              <c:f>SN9_RunTime!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Dekempeneer &amp; Derkinderen_x000d_(20 threads)</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Algoritme Codish et al. door_x000d_Dekempeneer &amp; Derkinderen_x000d_(20 threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Codish et al._x000d_(288 threads)</c:v>
                 </c:pt>
               </c:strCache>
@@ -923,14 +939,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SN9_RunTime!$B$2:$B$3</c:f>
+              <c:f>SN9_RunTime!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>4.204722</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>6.196933330409722</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>305.9666666666667</c:v>
                 </c:pt>
               </c:numCache>
@@ -947,11 +966,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="41"/>
-        <c:axId val="2125944208"/>
-        <c:axId val="2125947584"/>
+        <c:axId val="2098280736"/>
+        <c:axId val="2098233600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2125944208"/>
+        <c:axId val="2098280736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -989,7 +1008,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125947584"/>
+        <c:crossAx val="2098233600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -997,7 +1016,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125947584"/>
+        <c:axId val="2098233600"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1008,7 +1027,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125944208"/>
+        <c:crossAx val="2098280736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1110,6 +1129,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1209,6 +1229,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1229,13 +1250,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>SN9_RunTime!$A$2:$A$3</c:f>
+              <c:f>SN9_RunTime!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Dekempeneer &amp; Derkinderen_x000d_(20 threads)</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Algoritme Codish et al. door_x000d_Dekempeneer &amp; Derkinderen_x000d_(20 threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Codish et al._x000d_(288 threads)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1243,14 +1267,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SN9_RunTime!$B$2:$B$3</c:f>
+              <c:f>SN9_RunTime!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>4.204722</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>6.196933330409722</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>305.9666666666667</c:v>
                 </c:pt>
               </c:numCache>
@@ -1266,11 +1293,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="2125999552"/>
-        <c:axId val="2126002896"/>
+        <c:axId val="2134775696"/>
+        <c:axId val="2134742496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2125999552"/>
+        <c:axId val="2134775696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,7 +1340,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126002896"/>
+        <c:crossAx val="2134742496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1321,7 +1348,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126002896"/>
+        <c:axId val="2134742496"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1358,6 +1385,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1420,7 +1448,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125999552"/>
+        <c:crossAx val="2134775696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1434,6 +1462,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1510,6 +1539,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1572,13 +1602,16 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>SN9_RunTime!$A$2:$A$3</c:f>
+              <c:f>SN9_RunTime!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Dekempeneer &amp; Derkinderen_x000d_(20 threads)</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Algoritme Codish et al. door_x000d_Dekempeneer &amp; Derkinderen_x000d_(20 threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Codish et al._x000d_(288 threads)</c:v>
                 </c:pt>
               </c:strCache>
@@ -1586,14 +1619,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SN9_RunTime!$B$2:$B$3</c:f>
+              <c:f>SN9_RunTime!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>4.204722</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>6.196933330409722</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>305.9666666666667</c:v>
                 </c:pt>
               </c:numCache>
@@ -1610,11 +1646,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2126844320"/>
-        <c:axId val="2126847728"/>
+        <c:axId val="2131022384"/>
+        <c:axId val="2131025792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126844320"/>
+        <c:axId val="2131022384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1657,7 +1693,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126847728"/>
+        <c:crossAx val="2131025792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1665,7 +1701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126847728"/>
+        <c:axId val="2131025792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1718,7 +1754,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126844320"/>
+        <c:crossAx val="2131022384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1902,11 +1938,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2126892928"/>
-        <c:axId val="2126896320"/>
+        <c:axId val="2132326608"/>
+        <c:axId val="2132330000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126892928"/>
+        <c:axId val="2132326608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,7 +1985,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126896320"/>
+        <c:crossAx val="2132330000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1957,7 +1993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126896320"/>
+        <c:axId val="2132330000"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2009,7 +2045,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126892928"/>
+        <c:crossAx val="2132326608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2224,11 +2260,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2126934752"/>
-        <c:axId val="2126938144"/>
+        <c:axId val="2134882976"/>
+        <c:axId val="2133950368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126934752"/>
+        <c:axId val="2134882976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2271,7 +2307,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126938144"/>
+        <c:crossAx val="2133950368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2279,7 +2315,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126938144"/>
+        <c:axId val="2133950368"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2331,7 +2367,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126934752"/>
+        <c:crossAx val="2134882976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2659,11 +2695,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="2126983184"/>
-        <c:axId val="2126986512"/>
+        <c:axId val="2098207680"/>
+        <c:axId val="2098212960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126983184"/>
+        <c:axId val="2098207680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2706,7 +2742,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126986512"/>
+        <c:crossAx val="2098212960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2714,7 +2750,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126986512"/>
+        <c:axId val="2098212960"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2814,7 +2850,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126983184"/>
+        <c:crossAx val="2098207680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2905,6 +2941,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3127,11 +3164,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2127031584"/>
-        <c:axId val="2127034912"/>
+        <c:axId val="2131033648"/>
+        <c:axId val="2131036976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127031584"/>
+        <c:axId val="2131033648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3174,7 +3211,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127034912"/>
+        <c:crossAx val="2131036976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3182,7 +3219,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127034912"/>
+        <c:axId val="2131036976"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3234,7 +3271,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127031584"/>
+        <c:crossAx val="2131033648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3248,6 +3285,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7796,7 +7834,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="109" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7807,7 +7845,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7818,7 +7856,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7851,7 +7889,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7862,7 +7900,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7900,7 +7938,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9321101" cy="6082018"/>
+    <xdr:ext cx="9303008" cy="6071220"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -7927,7 +7965,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9321101" cy="6082018"/>
+    <xdr:ext cx="9303008" cy="6071220"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -7954,7 +7992,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9321101" cy="6082018"/>
+    <xdr:ext cx="9303008" cy="6071220"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -8035,7 +8073,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9321101" cy="6082018"/>
+    <xdr:ext cx="9303008" cy="6071220"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -8062,7 +8100,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309340" cy="6074434"/>
+    <xdr:ext cx="9303008" cy="6071220"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -8874,10 +8912,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8920,25 +8958,44 @@
         <v>15136.9992</v>
       </c>
       <c r="F2" s="14">
-        <f>D2/D3</f>
+        <f>D2/D4</f>
         <v>1.3742418564113738E-2</v>
       </c>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="15">
+        <f>C3/60</f>
+        <v>6.1969333304097223</v>
+      </c>
+      <c r="C3" s="15">
+        <f>D3/60</f>
+        <v>371.81599982458334</v>
+      </c>
+      <c r="D3" s="15">
+        <f>22308959989475/1000000000</f>
+        <v>22308.959989474999</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B4" s="15">
         <f>(7*24 + 17 + 58/60) + 5*24</f>
         <v>305.9666666666667</v>
       </c>
-      <c r="C3" s="15">
-        <f>$B3*60</f>
+      <c r="C4" s="15">
+        <f>$B4*60</f>
         <v>18358</v>
       </c>
-      <c r="D3" s="15">
-        <f>$C3*60</f>
+      <c r="D4" s="15">
+        <f>$C4*60</f>
         <v>1101480</v>
       </c>
     </row>

</xml_diff>